<commit_message>
Bugfix anzahlRubine werden bei next level vom FMENU nicht resetet
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\BlueJ\RubyRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{253DE2C0-03B7-4046-89E6-C37A09288824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCAA25F-ECE0-4B93-926E-9CC727F98535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3315" yWindow="2865" windowWidth="6660" windowHeight="9885" xr2:uid="{0227E2C2-B94F-4828-9A3E-CD9003934140}"/>
+    <workbookView xWindow="2265" yWindow="5160" windowWidth="5985" windowHeight="8025" xr2:uid="{0227E2C2-B94F-4828-9A3E-CD9003934140}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Objekt</t>
   </si>
@@ -75,7 +75,10 @@
     <t>Weg</t>
   </si>
   <si>
-    <t>Schlange</t>
+    <t>Schlange Y</t>
+  </si>
+  <si>
+    <t>Schlange X</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F81493-BFB4-4A7A-88DE-E10D619A3B7A}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,41 +538,41 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D8">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -577,21 +580,35 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>255</v>
+      </c>
+      <c r="C11">
+        <v>115</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>150</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>150</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>150</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A11">
-    <sortCondition ref="A2:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Teleportsteine sind vorhanden, aber noch keine Funktion
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\BlueJ\RubyRun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninam\OneDrive\Desktop\Programmieren\Ruby_Run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCAA25F-ECE0-4B93-926E-9CC727F98535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="5160" windowWidth="5985" windowHeight="8025" xr2:uid="{0227E2C2-B94F-4828-9A3E-CD9003934140}"/>
+    <workbookView xWindow="2268" yWindow="5160" windowWidth="5988" windowHeight="8028"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Objekt</t>
   </si>
@@ -79,12 +78,18 @@
   </si>
   <si>
     <t>Schlange X</t>
+  </si>
+  <si>
+    <t>TeleA</t>
+  </si>
+  <si>
+    <t>TeleB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,16 +434,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F81493-BFB4-4A7A-88DE-E10D619A3B7A}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -466,7 +471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -480,7 +485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -494,7 +499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -508,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -522,7 +527,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -536,7 +541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -550,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -564,7 +569,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -578,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -592,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -606,8 +611,36 @@
         <v>150</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>250</v>
+      </c>
+      <c r="C13">
+        <v>250</v>
+      </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>200</v>
+      </c>
+      <c r="C14">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+  <sortState ref="A2:D12">
     <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementierung Schlüssel Bugfix Schlangen machen kein Damage bei Bewwgung Bugfix Saphire konnten nicht aufgesammelt werden
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninam\OneDrive\Desktop\Programmieren\Ruby_Run\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\BlueJ\RubyRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965A76A8-0A37-4E09-B4B7-3B11EF0FDC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="5160" windowWidth="5988" windowHeight="8028"/>
+    <workbookView xWindow="2265" yWindow="5160" windowWidth="5985" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Objekt</t>
   </si>
@@ -84,12 +76,15 @@
   </si>
   <si>
     <t>TeleB</t>
+  </si>
+  <si>
+    <t>Schlüssel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,16 +429,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -471,7 +466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -485,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -499,7 +494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -513,7 +508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -527,7 +522,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -541,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -555,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -569,7 +564,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -583,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -597,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -611,7 +606,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -625,7 +620,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -639,8 +634,22 @@
         <v>200</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:D12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
     <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Schlüssel und Schloss/tür fertig TODO: Schlüssel & Schloss dynamisch anlegen da aktuell nur 1x pro level möglich!
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\BlueJ\RubyRun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965A76A8-0A37-4E09-B4B7-3B11EF0FDC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279F8D03-8633-4DFE-A5D8-143AA227CCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2265" yWindow="5160" windowWidth="5985" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Objekt</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Schlüssel</t>
+  </si>
+  <si>
+    <t>Schloss für Schlüssel</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +649,20 @@
       </c>
       <c r="D15">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bossgraphiken, tutoriallevel, auskommentiertes versuch für bosslevel umsetzung
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\BlueJ\RubyRun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ninam\OneDrive\Desktop\Programmieren\Ruby_Run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279F8D03-8633-4DFE-A5D8-143AA227CCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="5160" windowWidth="5985" windowHeight="8025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="5160" windowWidth="5988" windowHeight="8028"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Objekt</t>
   </si>
@@ -82,12 +81,27 @@
   </si>
   <si>
     <t>Schloss für Schlüssel</t>
+  </si>
+  <si>
+    <t>WandBoss</t>
+  </si>
+  <si>
+    <t>WegBoss</t>
+  </si>
+  <si>
+    <t>SteinBoss</t>
+  </si>
+  <si>
+    <t>RubinBoss</t>
+  </si>
+  <si>
+    <t>BuschBoss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,16 +446,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -469,7 +483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -483,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -497,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -511,7 +525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -525,7 +539,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -539,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -553,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -567,7 +581,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -581,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -595,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -609,7 +623,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -623,7 +637,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -637,7 +651,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -651,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -665,8 +679,78 @@
         <v>2</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>150</v>
+      </c>
+      <c r="C18">
+        <v>250</v>
+      </c>
+      <c r="D18">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>75</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+      <c r="D21">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D12">
+  <sortState ref="A2:D12">
     <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feuer wie Schlangenbewegung, sonst ohne Funktion
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Objekt</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>SchlangeBoss</t>
+  </si>
+  <si>
+    <t>Feuer</t>
+  </si>
+  <si>
+    <t>feuer Y</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,6 +770,34 @@
       </c>
       <c r="D22">
         <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>400</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>400</v>
+      </c>
+      <c r="C24">
+        <v>150</v>
+      </c>
+      <c r="D24">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Levelanpassungen, kein lvl sieben und vier(bzw ist das gleiche wie eins)
</commit_message>
<xml_diff>
--- a/RGB Werte.xlsx
+++ b/RGB Werte.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Objekt</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>feuer Y</t>
+  </si>
+  <si>
+    <t>AusgangRechts</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,6 +801,20 @@
       </c>
       <c r="D24">
         <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>255</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>